<commit_message>
Más casos de prueba
</commit_message>
<xml_diff>
--- a/docs/Casos de Prueba.xlsx
+++ b/docs/Casos de Prueba.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galla\PycharmProjects\G81.2022.14.FP\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E5DE2D-4F4B-4A05-8685-B078A4E38BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="76">
   <si>
     <t>I/O</t>
   </si>
@@ -230,30 +239,41 @@
   </si>
   <si>
     <t>TEST_16</t>
+  </si>
+  <si>
+    <t>TEST_17</t>
+  </si>
+  <si>
+    <t>Cita ya cancelada</t>
+  </si>
+  <si>
+    <t>Comprobar si la cita ya ha sido cancelada anteriormente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -263,7 +283,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -285,44 +305,47 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -512,29 +535,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="13.5"/>
-    <col customWidth="1" min="4" max="4" width="13.13"/>
-    <col customWidth="1" min="6" max="6" width="20.13"/>
-    <col customWidth="1" min="7" max="7" width="46.88"/>
-    <col customWidth="1" min="8" max="8" width="58.38"/>
-    <col customWidth="1" min="9" max="9" width="17.88"/>
-    <col customWidth="1" min="10" max="10" width="76.5"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="46.88671875" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="76.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +598,7 @@
       </c>
       <c r="L1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -605,7 +633,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -640,7 +668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -675,7 +703,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -710,7 +738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -745,7 +773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -780,7 +808,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -815,7 +843,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -841,7 +869,7 @@
         <v>18</v>
       </c>
       <c r="I9" s="5">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>20</v>
@@ -850,7 +878,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -885,7 +913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -920,7 +948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -955,7 +983,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -990,7 +1018,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1025,7 +1053,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1060,7 +1088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1089,13 +1117,48 @@
         <v>19</v>
       </c>
       <c r="J16" s="5">
-        <v>210.0</v>
+        <v>210</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Caso de prueba fichero empty
</commit_message>
<xml_diff>
--- a/docs/Casos de Prueba.xlsx
+++ b/docs/Casos de Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galla\PycharmProjects\G81.2022.14.FP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E5DE2D-4F4B-4A05-8685-B078A4E38BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF46A05-4EA5-4AA3-AA75-D56562B260EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
   <si>
     <t>I/O</t>
   </si>
@@ -248,6 +248,21 @@
   </si>
   <si>
     <t>Comprobar si la cita ya ha sido cancelada anteriormente</t>
+  </si>
+  <si>
+    <t>fichero</t>
+  </si>
+  <si>
+    <t>TEST_18</t>
+  </si>
+  <si>
+    <t>Fichero facío</t>
+  </si>
+  <si>
+    <t>Comprobar si hay datos en el fichero</t>
+  </si>
+  <si>
+    <t>NONE</t>
   </si>
 </sst>
 </file>
@@ -545,10 +560,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -598,7 +613,7 @@
       </c>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -633,7 +648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -668,7 +683,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -703,7 +718,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -738,7 +753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -773,7 +788,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -808,7 +823,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -843,7 +858,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -878,7 +893,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -913,7 +928,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -948,7 +963,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -983,7 +998,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1018,7 +1033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1053,7 +1068,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1088,7 +1103,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1155,6 +1170,41 @@
         <v>20</v>
       </c>
       <c r="K17" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Casos de prueba de Pruebas Funcionales y mejora del Árbol de Derivación
</commit_message>
<xml_diff>
--- a/docs/Casos de Prueba.xlsx
+++ b/docs/Casos de Prueba.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galla\PycharmProjects\G81.2022.14.FP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF46A05-4EA5-4AA3-AA75-D56562B260EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{045E5496-DD2F-409E-AF1D-27149E2D309F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
+    <sheet name="CE y Valores Límites" sheetId="1" r:id="rId1"/>
+    <sheet name="Pruebas Estructurales" sheetId="2" r:id="rId2"/>
+    <sheet name="Pruebas Funcionales" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="286">
   <si>
     <t>I/O</t>
   </si>
@@ -263,13 +265,900 @@
   </si>
   <si>
     <t>NONE</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>NODE</t>
+  </si>
+  <si>
+    <t>TERMINAL (T) / NO TERMINAL (NT)</t>
+  </si>
+  <si>
+    <t>TYPE (DUPLICATION / DELETION / MODIFICATION / VALID)</t>
+  </si>
+  <si>
+    <t>FILE PATH</t>
+  </si>
+  <si>
+    <t>FILE CONTENT</t>
+  </si>
+  <si>
+    <t>EXPECTED RESULT</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>test_ok.json</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Final",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Todos los campos válidos</t>
+  </si>
+  <si>
+    <t>TEST_0</t>
+  </si>
+  <si>
+    <t>DELETION</t>
+  </si>
+  <si>
+    <t>MODIFICATION</t>
+  </si>
+  <si>
+    <t>DUPLICATION</t>
+  </si>
+  <si>
+    <t>Borramos nodo 1</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 1</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 1</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>{{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Final",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Final",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Final",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>TEST_5</t>
+  </si>
+  <si>
+    <t>TEST_19</t>
+  </si>
+  <si>
+    <t>TEST_20</t>
+  </si>
+  <si>
+    <t>TEST_21</t>
+  </si>
+  <si>
+    <t>TEST_22</t>
+  </si>
+  <si>
+    <t>TEST_23</t>
+  </si>
+  <si>
+    <t>TEST_24</t>
+  </si>
+  <si>
+    <t>TEST_25</t>
+  </si>
+  <si>
+    <t>TEST_26</t>
+  </si>
+  <si>
+    <t>TEST_27</t>
+  </si>
+  <si>
+    <t>TEST_28</t>
+  </si>
+  <si>
+    <t>TEST_29</t>
+  </si>
+  <si>
+    <t>TEST_30</t>
+  </si>
+  <si>
+    <t>TEST_31</t>
+  </si>
+  <si>
+    <t>TEST_32</t>
+  </si>
+  <si>
+    <t>TEST_33</t>
+  </si>
+  <si>
+    <t>TEST_34</t>
+  </si>
+  <si>
+    <t>TEST_35</t>
+  </si>
+  <si>
+    <t>TEST_36</t>
+  </si>
+  <si>
+    <t>TEST_37</t>
+  </si>
+  <si>
+    <t>TEST_38</t>
+  </si>
+  <si>
+    <t>TEST_39</t>
+  </si>
+  <si>
+    <t>TEST_40</t>
+  </si>
+  <si>
+    <t>TEST_41</t>
+  </si>
+  <si>
+    <t>TEST_42</t>
+  </si>
+  <si>
+    <t>TEST_43</t>
+  </si>
+  <si>
+    <t>TEST_44</t>
+  </si>
+  <si>
+    <t>TEST_45</t>
+  </si>
+  <si>
+    <t>TEST_46</t>
+  </si>
+  <si>
+    <t>TEST_47</t>
+  </si>
+  <si>
+    <t>TEST_48</t>
+  </si>
+  <si>
+    <t>TEST_49</t>
+  </si>
+  <si>
+    <t>TEST_50</t>
+  </si>
+  <si>
+    <t>TEST_51</t>
+  </si>
+  <si>
+    <t>TEST_52</t>
+  </si>
+  <si>
+    <t>TEST_53</t>
+  </si>
+  <si>
+    <t>TEST_54</t>
+  </si>
+  <si>
+    <t>TEST_55</t>
+  </si>
+  <si>
+    <t>TEST_56</t>
+  </si>
+  <si>
+    <t>TEST_57</t>
+  </si>
+  <si>
+    <t>TEST_58</t>
+  </si>
+  <si>
+    <t>TEST_59</t>
+  </si>
+  <si>
+    <t>TEST_60</t>
+  </si>
+  <si>
+    <t>TEST_61</t>
+  </si>
+  <si>
+    <t>TEST_62</t>
+  </si>
+  <si>
+    <t>TEST_63</t>
+  </si>
+  <si>
+    <t>TEST_64</t>
+  </si>
+  <si>
+    <t>TEST_65</t>
+  </si>
+  <si>
+    <t>TEST_66</t>
+  </si>
+  <si>
+    <t>TEST_67</t>
+  </si>
+  <si>
+    <t>Borramos nodo 3</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 3</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 3</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 4</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 4</t>
+  </si>
+  <si>
+    <t>Borramos nodo 5</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 5</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 5</t>
+  </si>
+  <si>
+    <t>Borramos nodo 6</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 6</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 6</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>&amp;
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    }</t>
+  </si>
+  <si>
+    <t>{
+    XD
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist" "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Borramos nodo 11</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 11</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  </t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  &amp;</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }}</t>
+  </si>
+  <si>
+    <t>{
+    ",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    &amp;,
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c"  "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Borramos nodo 15|19</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 15|19</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 15|19</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c"
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c"&amp;
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",,
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Borramos nodo 8</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 8</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 8</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+   ,
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+   &amp;,
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal"  "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Borramos nodo 10</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 10</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 10</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+   &amp;
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist" "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Borramos nodo 12</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 12</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 12</t>
+  </si>
+  <si>
+    <t>{
+   : "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    &amp;: "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature""_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>23,24,25</t>
+  </si>
+  <si>
+    <t>23,24,26</t>
+  </si>
+  <si>
+    <t>23,24,27</t>
+  </si>
+  <si>
+    <t>Borramos nodo 23|24|25</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 23|24|25</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 23|24|25</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature" "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type"&amp; "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason" "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Borramos nodo 14</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 14</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": ,
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": &amp;,
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c""5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 16</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 16</t>
+  </si>
+  <si>
+    <t>Borramos nodo 16</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    : "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    &amp;: "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type""_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 18</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 18</t>
+  </si>
+  <si>
+    <t>Borramos nodo 18</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type":,
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": &amp;,
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal""Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 20</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 20</t>
+  </si>
+  <si>
+    <t>Borramos nodo 20</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    &amp;: "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    : "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason""_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 22</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 22</t>
+  </si>
+  <si>
+    <t>Borramos nodo 22</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": 
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": &amp;
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist""I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>34,36,37,37,40,42,52,54,55,57,58,60</t>
+  </si>
+  <si>
+    <t>{
+    _VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    &amp;_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    ""_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 59</t>
+  </si>
+  <si>
+    <t>Borramos nodo 59</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 35</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 35</t>
+  </si>
+  <si>
+    <t>Borramos nodo 35</t>
+  </si>
+  <si>
+    <t>{
+    "": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "&amp;": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 38</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 38</t>
+  </si>
+  <si>
+    <t>Borramos nodo 38</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "&amp;": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 41</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 41</t>
+  </si>
+  <si>
+    <t>Borramos nodo 41</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "&amp;": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 53</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 53</t>
+  </si>
+  <si>
+    <t>Borramos nodo 53</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "&amp;",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>Modificamos nodo 56</t>
+  </si>
+  <si>
+    <t>Duplicamos nodo 56</t>
+  </si>
+  <si>
+    <t>Borramos nodo 56</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "&amp;",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "TemporalTemporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": ""
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "&amp;"
+  }</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "5a06c7bede3d584e934e2f5bd3861e625cb31937f9f1a5362a51fbbf38486f1c",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentistI have to go to the dentist"
+  }</t>
+  </si>
+  <si>
+    <t>test_ok_final.json</t>
+  </si>
+  <si>
+    <t>TEST_68</t>
+  </si>
+  <si>
+    <t>Otro json</t>
+  </si>
+  <si>
+    <t>test_ok_second.json</t>
+  </si>
+  <si>
+    <t>{
+    "_VaccinationCancellationLog__date_signature": "6a8403d8605804cf2534fd7885940f3c3d8ec60ba578bc158b5dc2b9fb68d524",
+    "_VaccinationCancellationLog__type": "Temporal",
+    "_VaccinationCancellationLog__reason": "I have to go to the dentist"
+  }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -292,8 +1181,27 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,11 +1226,88 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -331,7 +1316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -341,6 +1326,49 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,7 +1590,7 @@
   </sheetPr>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -1211,4 +2239,2333 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AF4015-F0F8-49E8-899D-5104DAE8A3D0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A85A82-1FF8-4834-A27E-A0057D7D9DAD}">
+  <dimension ref="A1:O70"/>
+  <sheetViews>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="65.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="18"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+    </row>
+    <row r="3" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+    </row>
+    <row r="5" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+    </row>
+    <row r="6" spans="1:15" ht="145.19999999999999" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+    </row>
+    <row r="7" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+    </row>
+    <row r="9" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9">
+        <v>3</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+    </row>
+    <row r="11" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9">
+        <v>3</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" ht="132" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9">
+        <v>3</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9">
+        <v>11</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9">
+        <v>11</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+    </row>
+    <row r="15" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9">
+        <v>11</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" ht="66" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9">
+        <v>6</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+    </row>
+    <row r="17" spans="1:15" ht="66" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9">
+        <v>6</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+    </row>
+    <row r="18" spans="1:15" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>16</v>
+      </c>
+      <c r="B18" s="9">
+        <v>6</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+    </row>
+    <row r="19" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>17</v>
+      </c>
+      <c r="B19" s="9">
+        <v>15.19</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+    </row>
+    <row r="20" spans="1:15" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>18</v>
+      </c>
+      <c r="B20" s="9">
+        <v>15.19</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+    </row>
+    <row r="21" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>19</v>
+      </c>
+      <c r="B21" s="9">
+        <v>15.19</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+    </row>
+    <row r="22" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>20</v>
+      </c>
+      <c r="B22" s="9">
+        <v>8</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+    </row>
+    <row r="23" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>21</v>
+      </c>
+      <c r="B23" s="9">
+        <v>8</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+    </row>
+    <row r="24" spans="1:15" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24" s="9">
+        <v>8</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+    </row>
+    <row r="25" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>23</v>
+      </c>
+      <c r="B25" s="9">
+        <v>10</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+    </row>
+    <row r="26" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>24</v>
+      </c>
+      <c r="B26" s="9">
+        <v>10</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+    </row>
+    <row r="27" spans="1:15" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>25</v>
+      </c>
+      <c r="B27" s="9">
+        <v>10</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+    </row>
+    <row r="28" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>26</v>
+      </c>
+      <c r="B28" s="9">
+        <v>12</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+    </row>
+    <row r="29" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>27</v>
+      </c>
+      <c r="B29" s="9">
+        <v>12</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+    </row>
+    <row r="30" spans="1:15" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>28</v>
+      </c>
+      <c r="B30" s="9">
+        <v>12</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+    </row>
+    <row r="31" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>29</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+    </row>
+    <row r="32" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>30</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+    </row>
+    <row r="33" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>31</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+    </row>
+    <row r="34" spans="1:15" ht="66" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>32</v>
+      </c>
+      <c r="B34" s="11">
+        <v>14</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+    </row>
+    <row r="35" spans="1:15" ht="66" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>33</v>
+      </c>
+      <c r="B35" s="11">
+        <v>14</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+    </row>
+    <row r="36" spans="1:15" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>34</v>
+      </c>
+      <c r="B36" s="11">
+        <v>14</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+    </row>
+    <row r="37" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>35</v>
+      </c>
+      <c r="B37" s="11">
+        <v>16</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+    </row>
+    <row r="38" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>36</v>
+      </c>
+      <c r="B38" s="11">
+        <v>16</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+    </row>
+    <row r="39" spans="1:15" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>37</v>
+      </c>
+      <c r="B39" s="11">
+        <v>16</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+    </row>
+    <row r="40" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>38</v>
+      </c>
+      <c r="B40" s="11">
+        <v>18</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+    </row>
+    <row r="41" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>39</v>
+      </c>
+      <c r="B41" s="11">
+        <v>18</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+    </row>
+    <row r="42" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>40</v>
+      </c>
+      <c r="B42" s="11">
+        <v>18</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+    </row>
+    <row r="43" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>41</v>
+      </c>
+      <c r="B43" s="11">
+        <v>20</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+    </row>
+    <row r="44" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>42</v>
+      </c>
+      <c r="B44" s="11">
+        <v>20</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
+        <v>43</v>
+      </c>
+      <c r="B45" s="11">
+        <v>20</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>44</v>
+      </c>
+      <c r="B46" s="11">
+        <v>22</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
+        <v>45</v>
+      </c>
+      <c r="B47" s="11">
+        <v>22</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
+        <v>46</v>
+      </c>
+      <c r="B48" s="11">
+        <v>22</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
+        <v>47</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A50" s="9">
+        <v>48</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A51" s="9">
+        <v>49</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H51" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A52" s="9">
+        <v>50</v>
+      </c>
+      <c r="B52" s="11">
+        <v>35</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A53" s="9">
+        <v>51</v>
+      </c>
+      <c r="B53" s="11">
+        <v>35</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>52</v>
+      </c>
+      <c r="B54" s="11">
+        <v>35</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A55" s="9">
+        <v>53</v>
+      </c>
+      <c r="B55" s="11">
+        <v>38</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A56" s="9">
+        <v>54</v>
+      </c>
+      <c r="B56" s="11">
+        <v>38</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
+        <v>55</v>
+      </c>
+      <c r="B57" s="11">
+        <v>38</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A58" s="9">
+        <v>56</v>
+      </c>
+      <c r="B58" s="11">
+        <v>41</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H58" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>57</v>
+      </c>
+      <c r="B59" s="20">
+        <v>41</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H59" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A60" s="9">
+        <v>58</v>
+      </c>
+      <c r="B60" s="11">
+        <v>41</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H60" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
+        <v>59</v>
+      </c>
+      <c r="B61" s="11">
+        <v>53</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H61" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
+        <v>60</v>
+      </c>
+      <c r="B62" s="11">
+        <v>53</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="I62" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9">
+        <v>61</v>
+      </c>
+      <c r="B63" s="11">
+        <v>53</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A64" s="9">
+        <v>62</v>
+      </c>
+      <c r="B64" s="11">
+        <v>56</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="I64" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
+        <v>63</v>
+      </c>
+      <c r="B65" s="11">
+        <v>56</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H65" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
+        <v>64</v>
+      </c>
+      <c r="B66" s="11">
+        <v>56</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="I66" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
+        <v>65</v>
+      </c>
+      <c r="B67" s="11">
+        <v>59</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A68" s="9">
+        <v>66</v>
+      </c>
+      <c r="B68" s="11">
+        <v>59</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F68" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="I68" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A69" s="9">
+        <v>67</v>
+      </c>
+      <c r="B69" s="11">
+        <v>59</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A70" s="9">
+        <v>68</v>
+      </c>
+      <c r="B70" s="9">
+        <v>1</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Memoria y casos de prueba en Pruebas Estruturales
</commit_message>
<xml_diff>
--- a/docs/Casos de Prueba.xlsx
+++ b/docs/Casos de Prueba.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galla\PycharmProjects\G81.2022.14.FP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{045E5496-DD2F-409E-AF1D-27149E2D309F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31497D12-B1AB-46AA-B545-285CF4930E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CE y Valores Límites" sheetId="1" r:id="rId1"/>
-    <sheet name="Pruebas Estructurales" sheetId="2" r:id="rId2"/>
-    <sheet name="Pruebas Funcionales" sheetId="3" r:id="rId3"/>
+    <sheet name="Pruebas Funcionales" sheetId="3" r:id="rId2"/>
+    <sheet name="Pruebas Estructurales" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="298">
   <si>
     <t>I/O</t>
   </si>
@@ -1152,13 +1152,49 @@
     "_VaccinationCancellationLog__type": "Temporal",
     "_VaccinationCancellationLog__reason": "I have to go to the dentist"
   }</t>
+  </si>
+  <si>
+    <t>PATH</t>
+  </si>
+  <si>
+    <t>ID_TEST</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>Camino correcto, test válido</t>
+  </si>
+  <si>
+    <t>1-2-3-End</t>
+  </si>
+  <si>
+    <t>1-Error</t>
+  </si>
+  <si>
+    <t>1-2-Error</t>
+  </si>
+  <si>
+    <t>1-2-3-Error</t>
+  </si>
+  <si>
+    <t>VaccineException</t>
+  </si>
+  <si>
+    <t>Fallo al obtener cancellación del Json</t>
+  </si>
+  <si>
+    <t>Fallo al obtener cita del date_signature</t>
+  </si>
+  <si>
+    <t>Fallo al registrar cancelación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1198,6 +1234,11 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1316,7 +1357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1368,6 +1409,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2242,22 +2289,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AF4015-F0F8-49E8-899D-5104DAE8A3D0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A85A82-1FF8-4834-A27E-A0057D7D9DAD}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -4568,4 +4603,129 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AF4015-F0F8-49E8-899D-5104DAE8A3D0}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>297</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>